<commit_message>
a..again - fixed prices for moving 2 bricks together again, made a mistake in the last fix
</commit_message>
<xml_diff>
--- a/runs.xlsx
+++ b/runs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ofir\eclipse-workspace\SolvingProblemsWithSearchAlgos_Task1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64ED9E-3ED6-4A82-A419-8F8BAADE76C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC2D62C-599B-4A90-B906-02F21081E566}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{D107853A-7777-4072-9384-ECFB2D69EAC6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="after" sheetId="1" r:id="rId1"/>
+    <sheet name="before fixing cost of 2 blocks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="35">
   <si>
     <t>Algo</t>
   </si>
@@ -115,6 +116,30 @@
   </si>
   <si>
     <t>killed it after 40 minutes</t>
+  </si>
+  <si>
+    <t>8R-11D-7L-8U</t>
+  </si>
+  <si>
+    <t>5D-3R-3U-2&amp;5U-7L-7L-5&amp;6D-4D-3R-2R-2U-4L-4L-5&amp;6U</t>
+  </si>
+  <si>
+    <t>5D-3R-3U-2&amp;5U-7L-7L-5&amp;6D-4D-2R-3R-2U-4L-4L-5&amp;6U</t>
+  </si>
+  <si>
+    <t>5D-3R-3U-2&amp;5U-7L-7L-5&amp;6D-2R-4D-3R-2U-4L-4L-5&amp;6U</t>
+  </si>
+  <si>
+    <t>4L-1U-6R-2U-6R-5D-3R-7D-7D-4L-1L-2U-3R-4D-1L-2L-3U-5&amp;6U</t>
+  </si>
+  <si>
+    <t>9&amp;10D-3R-3R-5D-6R-1U-1U-5&amp;9L-10L-6D-2L-3U-7L-8U</t>
+  </si>
+  <si>
+    <t>9&amp;10D-3R-1U-3R-5D-6R-1U-5&amp;9L-6D-2L-3U-7L-8U-10L</t>
+  </si>
+  <si>
+    <t>killed it after 20 minutes</t>
   </si>
 </sst>
 </file>
@@ -174,18 +199,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -502,10 +530,635 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF4C3C7-FAEE-4743-9601-87B8537F511C}">
+  <dimension ref="A1:R34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1E-3</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1E-3</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>1E-3</v>
+      </c>
+      <c r="H3">
+        <v>21</v>
+      </c>
+      <c r="I3">
+        <v>1E-3</v>
+      </c>
+      <c r="J3">
+        <v>35</v>
+      </c>
+      <c r="K3">
+        <v>1E-3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>178389</v>
+      </c>
+      <c r="C12">
+        <v>193.35</v>
+      </c>
+      <c r="D12">
+        <v>710253</v>
+      </c>
+      <c r="E12">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="F12">
+        <v>30803896</v>
+      </c>
+      <c r="G12">
+        <v>17.222000000000001</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12">
+        <v>95094019</v>
+      </c>
+      <c r="K12">
+        <v>45.252000000000002</v>
+      </c>
+      <c r="O12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="Q13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="Q14" t="s">
+        <v>3</v>
+      </c>
+      <c r="R14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="Q15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="Q16" t="s">
+        <v>5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="3"/>
+      <c r="M19" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21">
+        <v>4355083</v>
+      </c>
+      <c r="E21">
+        <v>2.528</v>
+      </c>
+      <c r="F21">
+        <v>1453420</v>
+      </c>
+      <c r="G21">
+        <v>1.173</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="O21" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="Q22" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="Q23" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="Q24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="Q25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="M28" t="s">
+        <v>13</v>
+      </c>
+      <c r="O28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>69967</v>
+      </c>
+      <c r="C30">
+        <v>29.241</v>
+      </c>
+      <c r="D30">
+        <v>318200</v>
+      </c>
+      <c r="E30">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="F30">
+        <v>289797584</v>
+      </c>
+      <c r="G30">
+        <v>157.96600000000001</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30">
+        <v>247533960</v>
+      </c>
+      <c r="K30">
+        <v>112.90600000000001</v>
+      </c>
+      <c r="O30" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>1</v>
+      </c>
+      <c r="R30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q31" t="s">
+        <v>2</v>
+      </c>
+      <c r="R31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q34" t="s">
+        <v>5</v>
+      </c>
+      <c r="R34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J28:K28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8403A5A5-3E34-48D6-9A87-3ECA2B12C3B5}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,29 +1171,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="3"/>
       <c r="M1" t="s">
         <v>8</v>
       </c>
@@ -549,35 +1202,35 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O2" t="s">
@@ -620,29 +1273,29 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="3"/>
       <c r="M6" t="s">
         <v>9</v>
       </c>
@@ -651,35 +1304,35 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O7" t="s">
@@ -705,10 +1358,10 @@
       <c r="G8">
         <v>15.462999999999999</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="2"/>
       <c r="J8">
         <v>95094019</v>
       </c>
@@ -720,29 +1373,29 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="1"/>
+      <c r="K10" s="3"/>
       <c r="M10" t="s">
         <v>11</v>
       </c>
@@ -751,35 +1404,35 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="3" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O11" t="s">
@@ -787,10 +1440,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="2"/>
       <c r="D12">
         <v>4116133</v>
       </c>
@@ -803,42 +1456,42 @@
       <c r="G12">
         <v>1.198</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="4"/>
+      <c r="K12" s="2"/>
       <c r="O12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="1" t="s">
+      <c r="C14" s="4"/>
+      <c r="D14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1" t="s">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="1"/>
+      <c r="K14" s="3"/>
       <c r="M14" t="s">
         <v>13</v>
       </c>
@@ -847,35 +1500,35 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15" s="3" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O15" t="s">
@@ -901,10 +1554,10 @@
       <c r="G16">
         <v>242.52699999999999</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="2"/>
       <c r="J16">
         <v>247533960</v>
       </c>
@@ -918,9 +1571,9 @@
   </sheetData>
   <mergeCells count="29">
     <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J10:K10"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J10:K10"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:C14"/>

</xml_diff>

<commit_message>
Added creation time to Node comparison. This was required and I forgot. Thanks Oriel.
</commit_message>
<xml_diff>
--- a/runs.xlsx
+++ b/runs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ofir\eclipse-workspace\SolvingProblemsWithSearchAlgos_Task1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC2D62C-599B-4A90-B906-02F21081E566}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A225D9-993B-4B38-9B83-707833D2F562}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{D107853A-7777-4072-9384-ECFB2D69EAC6}"/>
+    <workbookView xWindow="0" yWindow="4476" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{D107853A-7777-4072-9384-ECFB2D69EAC6}"/>
   </bookViews>
   <sheets>
-    <sheet name="after" sheetId="1" r:id="rId1"/>
-    <sheet name="before fixing cost of 2 blocks" sheetId="2" r:id="rId2"/>
+    <sheet name="after adding create time comapr" sheetId="3" r:id="rId1"/>
+    <sheet name="after fixing cost of 2 blocks" sheetId="1" r:id="rId2"/>
+    <sheet name="before fixing cost of 2 blocks" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="35">
   <si>
     <t>Algo</t>
   </si>
@@ -199,12 +200,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -213,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -529,11 +533,634 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928409DD-95D1-4A07-BB1D-3A8EFA5E12B0}">
+  <dimension ref="A1:R34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1E-3</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1E-3</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>2E-3</v>
+      </c>
+      <c r="H3">
+        <v>21</v>
+      </c>
+      <c r="I3">
+        <v>1E-3</v>
+      </c>
+      <c r="J3">
+        <v>35</v>
+      </c>
+      <c r="K3">
+        <v>1E-3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>180847</v>
+      </c>
+      <c r="C12">
+        <v>170.25700000000001</v>
+      </c>
+      <c r="D12">
+        <v>710253</v>
+      </c>
+      <c r="E12">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F12">
+        <v>30803896</v>
+      </c>
+      <c r="G12">
+        <v>16.294</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12">
+        <v>95094019</v>
+      </c>
+      <c r="K12">
+        <v>42.206000000000003</v>
+      </c>
+      <c r="O12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="Q13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="Q14" t="s">
+        <v>3</v>
+      </c>
+      <c r="R14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="Q15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="Q16" t="s">
+        <v>5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="M19" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21">
+        <v>4355083</v>
+      </c>
+      <c r="E21">
+        <v>2.2959999999999998</v>
+      </c>
+      <c r="F21">
+        <v>1454041</v>
+      </c>
+      <c r="G21">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="O21" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="Q22" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="Q23" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="Q24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="Q25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="M28" t="s">
+        <v>13</v>
+      </c>
+      <c r="O28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>83452</v>
+      </c>
+      <c r="C30">
+        <v>36.738</v>
+      </c>
+      <c r="D30">
+        <v>318200</v>
+      </c>
+      <c r="E30">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F30">
+        <v>289968774</v>
+      </c>
+      <c r="G30">
+        <v>160.97499999999999</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30">
+        <v>247533960</v>
+      </c>
+      <c r="K30">
+        <v>112.092</v>
+      </c>
+      <c r="O30" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>1</v>
+      </c>
+      <c r="R30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q31" t="s">
+        <v>2</v>
+      </c>
+      <c r="R31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q34" t="s">
+        <v>5</v>
+      </c>
+      <c r="R34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF4C3C7-FAEE-4743-9601-87B8537F511C}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:I21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,29 +1174,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3"/>
+      <c r="K1" s="4"/>
       <c r="M1" t="s">
         <v>8</v>
       </c>
@@ -578,7 +1205,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -687,29 +1314,29 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3" t="s">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="4"/>
       <c r="M10" t="s">
         <v>9</v>
       </c>
@@ -718,7 +1345,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -772,8 +1399,8 @@
       <c r="G12">
         <v>17.222000000000001</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
       <c r="J12">
         <v>95094019</v>
       </c>
@@ -791,8 +1418,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
       <c r="Q13" t="s">
         <v>2</v>
       </c>
@@ -801,8 +1428,8 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
       <c r="Q14" t="s">
         <v>3</v>
       </c>
@@ -811,15 +1438,15 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
       <c r="Q15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
       <c r="Q16" t="s">
         <v>5</v>
       </c>
@@ -828,33 +1455,33 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3" t="s">
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="3"/>
+      <c r="K19" s="4"/>
       <c r="M19" t="s">
         <v>11</v>
       </c>
@@ -863,7 +1490,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
@@ -899,10 +1526,10 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="6"/>
       <c r="D21">
         <v>4355083</v>
       </c>
@@ -915,10 +1542,10 @@
       <c r="G21">
         <v>1.173</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
       <c r="O21" t="s">
         <v>19</v>
       </c>
@@ -927,12 +1554,12 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
       <c r="Q22" t="s">
         <v>2</v>
       </c>
@@ -941,12 +1568,12 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
       <c r="Q23" t="s">
         <v>3</v>
       </c>
@@ -955,59 +1582,59 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
       <c r="Q24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
       <c r="Q25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3" t="s">
+      <c r="C28" s="5"/>
+      <c r="D28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3" t="s">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3" t="s">
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="3"/>
+      <c r="K28" s="4"/>
       <c r="M28" t="s">
         <v>13</v>
       </c>
@@ -1016,7 +1643,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1070,8 +1697,8 @@
       <c r="G30">
         <v>157.96600000000001</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
       <c r="J30">
         <v>247533960</v>
       </c>
@@ -1119,6 +1746,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -1131,29 +1775,12 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J28:K28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8403A5A5-3E34-48D6-9A87-3ECA2B12C3B5}">
   <dimension ref="A1:O16"/>
   <sheetViews>
@@ -1171,29 +1798,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3"/>
+      <c r="K1" s="4"/>
       <c r="M1" t="s">
         <v>8</v>
       </c>
@@ -1202,7 +1829,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1273,29 +1900,29 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="4"/>
       <c r="M6" t="s">
         <v>9</v>
       </c>
@@ -1304,7 +1931,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1358,10 +1985,10 @@
       <c r="G8">
         <v>15.462999999999999</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="6"/>
       <c r="J8">
         <v>95094019</v>
       </c>
@@ -1373,29 +2000,29 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3" t="s">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="4"/>
       <c r="M10" t="s">
         <v>11</v>
       </c>
@@ -1404,7 +2031,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1440,10 +2067,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="6"/>
       <c r="D12">
         <v>4116133</v>
       </c>
@@ -1456,42 +2083,42 @@
       <c r="G12">
         <v>1.198</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="6"/>
       <c r="O12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="s">
+      <c r="I14" s="4"/>
+      <c r="J14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="4"/>
       <c r="M14" t="s">
         <v>13</v>
       </c>
@@ -1500,7 +2127,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1554,10 +2181,10 @@
       <c r="G16">
         <v>242.52699999999999</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="6"/>
       <c r="J16">
         <v>247533960</v>
       </c>
@@ -1570,28 +2197,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -1599,6 +2204,28 @@
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed created time of Nodes to Nano-seconds. Milli was too small (several nodes can be created within 1 milli). Thanks again to Oriel. Hopefully actually done.
</commit_message>
<xml_diff>
--- a/runs.xlsx
+++ b/runs.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ofir\eclipse-workspace\SolvingProblemsWithSearchAlgos_Task1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A225D9-993B-4B38-9B83-707833D2F562}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92158DDB-466B-4CF9-BB43-37A8DCF7D462}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4476" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{D107853A-7777-4072-9384-ECFB2D69EAC6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{D107853A-7777-4072-9384-ECFB2D69EAC6}"/>
   </bookViews>
   <sheets>
-    <sheet name="after adding create time comapr" sheetId="3" r:id="rId1"/>
-    <sheet name="after fixing cost of 2 blocks" sheetId="1" r:id="rId2"/>
-    <sheet name="before fixing cost of 2 blocks" sheetId="2" r:id="rId3"/>
+    <sheet name="timeNano" sheetId="4" r:id="rId1"/>
+    <sheet name="after adding create time comapr" sheetId="3" r:id="rId2"/>
+    <sheet name="after fixing cost of 2 blocks" sheetId="1" r:id="rId3"/>
+    <sheet name="before fixing cost of 2 blocks" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="35">
   <si>
     <t>Algo</t>
   </si>
@@ -200,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,13 +213,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,11 +537,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928409DD-95D1-4A07-BB1D-3A8EFA5E12B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8447C42-E901-485A-A1A1-8F4E8F0FFD4A}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,29 +555,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="6"/>
       <c r="M1" t="s">
         <v>8</v>
       </c>
@@ -582,35 +586,35 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O2" t="s">
@@ -634,7 +638,7 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="H3">
         <v>21</v>
@@ -691,29 +695,29 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="4"/>
+      <c r="K10" s="6"/>
       <c r="M10" t="s">
         <v>9</v>
       </c>
@@ -722,35 +726,35 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O11" t="s">
@@ -762,27 +766,27 @@
         <v>180847</v>
       </c>
       <c r="C12">
-        <v>170.25700000000001</v>
+        <v>187.626</v>
       </c>
       <c r="D12">
         <v>710253</v>
       </c>
       <c r="E12">
-        <v>0.47499999999999998</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="F12">
-        <v>30803896</v>
+        <v>710253</v>
       </c>
       <c r="G12">
-        <v>16.294</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+        <v>0.85</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="J12">
         <v>95094019</v>
       </c>
       <c r="K12">
-        <v>42.206000000000003</v>
+        <v>54.764000000000003</v>
       </c>
       <c r="O12" t="s">
         <v>25</v>
@@ -811,7 +815,7 @@
         <v>3</v>
       </c>
       <c r="R14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -836,29 +840,29 @@
       <c r="I17" s="3"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4" t="s">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4" t="s">
+      <c r="I19" s="6"/>
+      <c r="J19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="6"/>
       <c r="M19" t="s">
         <v>11</v>
       </c>
@@ -867,35 +871,35 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K20" s="2" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O20" t="s">
@@ -903,24 +907,24 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
       <c r="D21">
         <v>4355083</v>
       </c>
       <c r="E21">
-        <v>2.2959999999999998</v>
+        <v>3.198</v>
       </c>
       <c r="F21">
-        <v>1454041</v>
+        <v>1559622</v>
       </c>
       <c r="G21">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+        <v>1.4610000000000001</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
       <c r="O21" t="s">
         <v>19</v>
       </c>
@@ -987,29 +991,29 @@
       <c r="K26" s="3"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4" t="s">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4" t="s">
+      <c r="I28" s="6"/>
+      <c r="J28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="4"/>
+      <c r="K28" s="6"/>
       <c r="M28" t="s">
         <v>13</v>
       </c>
@@ -1018,35 +1022,35 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K29" s="2" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="O29" t="s">
@@ -1058,27 +1062,27 @@
         <v>83452</v>
       </c>
       <c r="C30">
-        <v>36.738</v>
+        <v>47.634999999999998</v>
       </c>
       <c r="D30">
         <v>318200</v>
       </c>
       <c r="E30">
-        <v>0.26400000000000001</v>
+        <v>0.438</v>
       </c>
       <c r="F30">
-        <v>289968774</v>
+        <v>325821114</v>
       </c>
       <c r="G30">
-        <v>160.97499999999999</v>
-      </c>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+        <v>228.691</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
       <c r="J30">
         <v>247533960</v>
       </c>
       <c r="K30">
-        <v>112.092</v>
+        <v>154.37</v>
       </c>
       <c r="O30" t="s">
         <v>16</v>
@@ -1156,10 +1160,633 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928409DD-95D1-4A07-BB1D-3A8EFA5E12B0}">
+  <dimension ref="A1:R34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1E-3</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1E-3</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>2E-3</v>
+      </c>
+      <c r="H3">
+        <v>21</v>
+      </c>
+      <c r="I3">
+        <v>1E-3</v>
+      </c>
+      <c r="J3">
+        <v>35</v>
+      </c>
+      <c r="K3">
+        <v>1E-3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q5" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>180847</v>
+      </c>
+      <c r="C12">
+        <v>170.25700000000001</v>
+      </c>
+      <c r="D12">
+        <v>710253</v>
+      </c>
+      <c r="E12">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F12">
+        <v>30803896</v>
+      </c>
+      <c r="G12">
+        <v>16.294</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12">
+        <v>95094019</v>
+      </c>
+      <c r="K12">
+        <v>42.206000000000003</v>
+      </c>
+      <c r="O12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="Q13" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="Q14" t="s">
+        <v>3</v>
+      </c>
+      <c r="R14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="Q15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="Q16" t="s">
+        <v>5</v>
+      </c>
+      <c r="R16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="6"/>
+      <c r="M19" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21">
+        <v>4355083</v>
+      </c>
+      <c r="E21">
+        <v>2.2959999999999998</v>
+      </c>
+      <c r="F21">
+        <v>1454041</v>
+      </c>
+      <c r="G21">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="O21" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="Q22" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="Q23" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="Q24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="Q25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="M28" t="s">
+        <v>13</v>
+      </c>
+      <c r="O28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>83452</v>
+      </c>
+      <c r="C30">
+        <v>36.738</v>
+      </c>
+      <c r="D30">
+        <v>318200</v>
+      </c>
+      <c r="E30">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F30">
+        <v>289968774</v>
+      </c>
+      <c r="G30">
+        <v>160.97499999999999</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30">
+        <v>247533960</v>
+      </c>
+      <c r="K30">
+        <v>112.092</v>
+      </c>
+      <c r="O30" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>1</v>
+      </c>
+      <c r="R30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q31" t="s">
+        <v>2</v>
+      </c>
+      <c r="R31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q32" t="s">
+        <v>3</v>
+      </c>
+      <c r="R32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="17:18" x14ac:dyDescent="0.3">
+      <c r="Q34" t="s">
+        <v>5</v>
+      </c>
+      <c r="R34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J28:K28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF4C3C7-FAEE-4743-9601-87B8537F511C}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -1174,29 +1801,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="6"/>
       <c r="M1" t="s">
         <v>8</v>
       </c>
@@ -1205,7 +1832,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1314,29 +1941,29 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="4"/>
+      <c r="K10" s="6"/>
       <c r="M10" t="s">
         <v>9</v>
       </c>
@@ -1345,7 +1972,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1399,8 +2026,8 @@
       <c r="G12">
         <v>17.222000000000001</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="J12">
         <v>95094019</v>
       </c>
@@ -1459,29 +2086,29 @@
       <c r="I17" s="3"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4" t="s">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4" t="s">
+      <c r="I19" s="6"/>
+      <c r="J19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="6"/>
       <c r="M19" t="s">
         <v>11</v>
       </c>
@@ -1490,7 +2117,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
@@ -1526,10 +2153,10 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="5"/>
       <c r="D21">
         <v>4355083</v>
       </c>
@@ -1542,10 +2169,10 @@
       <c r="G21">
         <v>1.173</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
       <c r="O21" t="s">
         <v>19</v>
       </c>
@@ -1612,29 +2239,29 @@
       <c r="K26" s="3"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4" t="s">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4" t="s">
+      <c r="I28" s="6"/>
+      <c r="J28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="4"/>
+      <c r="K28" s="6"/>
       <c r="M28" t="s">
         <v>13</v>
       </c>
@@ -1643,7 +2270,7 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1697,8 +2324,8 @@
       <c r="G30">
         <v>157.96600000000001</v>
       </c>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
       <c r="J30">
         <v>247533960</v>
       </c>
@@ -1746,23 +2373,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -1775,12 +2385,29 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J28:K28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8403A5A5-3E34-48D6-9A87-3ECA2B12C3B5}">
   <dimension ref="A1:O16"/>
   <sheetViews>
@@ -1798,29 +2425,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="6"/>
       <c r="M1" t="s">
         <v>8</v>
       </c>
@@ -1829,7 +2456,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1900,29 +2527,29 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="6"/>
       <c r="M6" t="s">
         <v>9</v>
       </c>
@@ -1931,7 +2558,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1985,10 +2612,10 @@
       <c r="G8">
         <v>15.462999999999999</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="5"/>
       <c r="J8">
         <v>95094019</v>
       </c>
@@ -2000,29 +2627,29 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="4"/>
+      <c r="K10" s="6"/>
       <c r="M10" t="s">
         <v>11</v>
       </c>
@@ -2031,7 +2658,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -2067,10 +2694,10 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
       <c r="D12">
         <v>4116133</v>
       </c>
@@ -2083,42 +2710,42 @@
       <c r="G12">
         <v>1.198</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6" t="s">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="6"/>
+      <c r="K12" s="5"/>
       <c r="O12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4" t="s">
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="6"/>
       <c r="M14" t="s">
         <v>13</v>
       </c>
@@ -2127,7 +2754,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
@@ -2181,10 +2808,10 @@
       <c r="G16">
         <v>242.52699999999999</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="5"/>
       <c r="J16">
         <v>247533960</v>
       </c>
@@ -2197,6 +2824,23 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -2209,23 +2853,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>